<commit_message>
KARMEN-5 reconstructed all P1 and P2 files based on the analysts. Technical checks were done and the files were sent to KARMEN.
</commit_message>
<xml_diff>
--- a/rmonize/data_dictionary/DD_KARMEN_P1.xlsx
+++ b/rmonize/data_dictionary/DD_KARMEN_P1.xlsx
@@ -352,7 +352,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -391,7 +391,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ID of the participant</t>
+          <t>ID</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -491,7 +491,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Energy intake [kcal/d]</t>
+          <t>Energy – incl. energy from dietary fiber</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -526,7 +526,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Gem02_1</t>
+          <t>Gem02_1_NCI</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -546,7 +546,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Gem02_2</t>
+          <t>Gem02_2_NCI</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -566,7 +566,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Gem02_Hu</t>
+          <t>Gem02_Hu_NCI</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -586,7 +586,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Obst_sum</t>
+          <t>Obst_sum_NCI</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -606,7 +606,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Nusa_sum</t>
+          <t>Nusa_sum_NCI</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -626,7 +626,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Milc_sum</t>
+          <t>Milc_sum_NCI</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -646,12 +646,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Milc07_1</t>
+          <t>milk_NCI</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Milk and dairy products including cocoa drinks, milkshakes, yoghurt, (sour) cream, buttermilk, kefir, whey, milk powder</t>
+          <t>Milk</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -666,12 +666,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Fermented_milk_NCI</t>
+          <t>milkbased_bev_NCI</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Fermented milk products</t>
+          <t>milk-based beverages incl. cocoa drinks, milkshakes</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -686,12 +686,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Milc07_2</t>
+          <t>Fermented_milk_NCI</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Cheese and curd cheese</t>
+          <t>Fermented milk products</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -706,12 +706,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Sues13_6</t>
+          <t>quark_curd_NCI</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Creams and desserts including pudding, semolina, tiramisu</t>
+          <t>quark and curd cheese</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -726,12 +726,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Brot_sum</t>
+          <t>cheeses_NCI</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Sum of Wholemeal bread/rolls, White, brown or multigrain bread/rolls, Cereals and cereal products, Pastries</t>
+          <t>Cheese</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -746,12 +746,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Flours_milled_prod_NCI</t>
+          <t>Sues13_6_NCI</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Flours, milled products</t>
+          <t>Creams and desserts including pudding, semolina, tiramisu</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -766,12 +766,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Pasta_rice_NCI</t>
+          <t>Brot_sum_NCI</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Pasta, rice</t>
+          <t>Sum of whole grain bread/rolls, White, brown or multigrain bread/rolls, Cereals and cereal products, Pastries</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -786,12 +786,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Brot01_1</t>
+          <t>Flours_milled_prod_NCI</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Sum of Wholemeal bread/rolls, White, brown or multigrain bread/rolls (incl. Crisp bread)</t>
+          <t>Flours, milled products</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -806,12 +806,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Bread_NCI</t>
+          <t>Pasta_rice_NCI</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Bread</t>
+          <t>Pasta, rice</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -826,12 +826,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Crispbread_NCI</t>
+          <t>Brot01_1_NCI</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Crispbread</t>
+          <t>Sum of Wholemeal bread/rolls, White, brown or multigrain bread/rolls (incl. Crisp bread)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -846,12 +846,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Breakfast_cereals_NCI</t>
+          <t>Bread_NCI</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Breakfast cereals</t>
+          <t>Bread</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -866,12 +866,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Crackers_NCI</t>
+          <t>Crispbread_NCI</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Crackers, breadsticks</t>
+          <t>Crispbread</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -886,12 +886,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Fine_bakery_NCI</t>
+          <t>Breakfast_cereals_NCI</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Fine bakery wares</t>
+          <t>Breakfast cereals</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -906,12 +906,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Flei_sum</t>
+          <t>Crackers_NCI</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Sum of meat and meat products unsmoked (including roast, goulash, schnitzel, beef olive, minced meat, meat balls, ground meat sauce) &amp; sausages and meat products smoked (including salami, liver sausage, ham, bacon, cured pork, meat loaf, bratwurst)</t>
+          <t>Crackers, breadsticks</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -926,12 +926,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Flei_Wurst</t>
+          <t>Fine_bakery_NCI</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Sausages and meat products smoked including salami, liver sausage, ham, bacon, cured pork, meat loaf, bratwurst</t>
+          <t>Fine bakery wares</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -946,12 +946,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Fish_sum</t>
+          <t>Flei_sum_NCI</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Fish and fish products including salt- and freshwater fish, shrimps, mussels, snails, processed products like caviar, tinned fish</t>
+          <t>Sum of meat and meat products unsmoked (including roast, goulash, schnitzel, beef olive, minced meat, meat balls, ground meat sauce) &amp; sausages and meat products smoked (including salami, liver sausage, ham, bacon, cured pork, meat loaf, bratwurst)</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -966,12 +966,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Eier_sum_NCI</t>
+          <t>Flei_Wurst_NCI</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Eggs and egg products including scrambled, fried and boiled eggs, omelets, soufflé</t>
+          <t>Sausages and meat products smoked including salami, liver sausage, ham, bacon, cured pork, meat loaf, bratwurst</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -986,12 +986,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Fett_sum</t>
+          <t>Fish_sum_NCI</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>fats &amp; oils (excl: in salad dressings) - incl. Animal-based fats, plant-based fats and not specified fats/öls</t>
+          <t>Fish and fish products including salt- and freshwater fish, shrimps, mussels, snails, processed products like caviar, tinned fish</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1006,12 +1006,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>veg_fatsoils_NCI</t>
+          <t>Eier_sum_NCI</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Vegetable fats and oils</t>
+          <t>Eggs and egg products including scrambled, fried and boiled eggs, omelets, soufflé</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1026,12 +1026,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Butter_NCI</t>
+          <t>Fett_sum_NCI</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Butter</t>
+          <t>fats &amp; oils (excl: in salad dressings) - incl. Animal-based fats, plant-based fats and not specified fats/oils</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1046,12 +1046,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Marg_Streichf_NCI</t>
+          <t>veg_fatsoils_NCI</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Margarine and similar</t>
+          <t>Vegetable fats and oils</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1066,12 +1066,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Animal_fatsoils_NCI</t>
+          <t>Butter_NCI</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Animal fats excluding butter, fish oil</t>
+          <t>Butter</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1086,12 +1086,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Sues_sum</t>
+          <t>Marg_Streichf_NCI</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Sweets (sum)</t>
+          <t>Margarine and similar</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1106,12 +1106,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Sues13_1</t>
+          <t>Animal_fatsoils_NCI</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Sweets including sweets with chocolate, confectionaries, candies, fruit gums, cereal bars</t>
+          <t>Animal fats excluding butter, fish oil</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1126,12 +1126,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Sues13_2</t>
+          <t>Sues_sum_NCI</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Ice cream</t>
+          <t>Sweets (sum)</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1146,12 +1146,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Cakes_NCI</t>
+          <t>chocolate_sweets_NCI</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Cakes</t>
+          <t>Sweets including chocolate, sweets with chocolate coating, confectioneries with chocolate</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1166,12 +1166,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Getr15_1</t>
+          <t>nonchoc_sweets_NCI</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>non-alcoholic beverages (sum)</t>
+          <t>Sweets without chocolate such as  candies, fruit gums, cereal bars</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1186,12 +1186,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Getr15_14</t>
+          <t>Sues13_2_NCI</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Fruit juices/nectars (incl. Spritzer) - excl. vegetable juices</t>
+          <t>Ice cream</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1206,12 +1206,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Getr15_16</t>
+          <t>Cakes_NCI</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Soft drinks e.g. lemonades, bitter lemon (incl. low-calorie drinks)</t>
+          <t>Cakes</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1226,12 +1226,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Getr15_11</t>
+          <t>Getr15_1_NCI</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Water</t>
+          <t>non-alcoholic beverages (sum)</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1246,12 +1246,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Getr15_12</t>
+          <t>Getr15_14_NCI</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Coffee + Tea (black/green)</t>
+          <t>Fruit juices/nectars (incl. Spritzer) - excl. vegetable juices</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1266,12 +1266,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Getr15_13</t>
+          <t>Getr15_16_NCI</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Herbal/fruit tea</t>
+          <t>Soft drinks e.g. lemonades, bitter lemon (incl. low-calorie drinks)</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1286,12 +1286,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Getr15_2</t>
+          <t>Getr15_11_NCI</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Alcoholic beverages (sum)</t>
+          <t>Water</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1306,12 +1306,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Getr15_22</t>
+          <t>blackgreentea_NCI</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Wine and sparkling wine</t>
+          <t>black and green tea</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1326,12 +1326,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Getr15_21</t>
+          <t>Kaffee_NCI</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Beer including mixed beer drinks</t>
+          <t>coffee</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1346,12 +1346,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Getr15_23</t>
+          <t>Getr15_13_NCI</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>spirits incl. schnapps, liqueurs</t>
+          <t>Herbal/fruit tea</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -1366,12 +1366,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Getr15_24</t>
+          <t>Getr15_2_NCI</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Other alcoholic beverages e.g. alcopops, cocktails</t>
+          <t>Alcoholic beverages (sum)</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -1386,12 +1386,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Sose_sum</t>
+          <t>Getr15_22_NCI</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Sauces including warm and cold sauces (e.g. ketchup, salad dressing), mustard, vinegar etc.; exceptions: fruit-, vegetable-, ground meat sauce</t>
+          <t>Wine and sparkling wine</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -1406,12 +1406,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Supp_sum</t>
+          <t>Getr15_21_NCI</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Soups without stews</t>
+          <t>Beer including mixed beer drinks</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1426,12 +1426,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Sonst_sum</t>
+          <t>Getr15_23_MW</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Milk substitutes (e.g. soy products (milk, yoghurt, cheese), coconut-, rice-, oat-, almond milk, cereal milk with soy), meat substitutes (e.g. tofu, tempeh, soy protein, vegetarian sausages), cereal substitutes (e.g. soy flour/flakes, lupines), sweeteners, sugar substitutes, beverage powders/ -granules (e.g. cocoa powder, lemonade powder), herbs, spices, vegetarian spreads, protein powder, yeast, miso</t>
+          <t>spirits incl. schnaps, liqueurs</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -1446,12 +1446,12 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Veg_products_NCI</t>
+          <t>Getr15_24_MW</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Vegetarian products</t>
+          <t>Other alcoholic beverages e.g. alcopops, cocktails</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -1466,12 +1466,12 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Soyproducts_NCI</t>
+          <t>Sose_sum_NCI</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Soyproducts</t>
+          <t>Sauces including warm and cold sauces (e.g. ketchup, salad dressing), mustard, vinegar etc.; exceptions: fruit-, vegetable-, ground meat sauce</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -1486,15 +1486,95 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Suessstoffe</t>
+          <t>Supp_sum_NCI</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
+          <t>Soups without stews</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Sonst_sum_NCI</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Milk substitutes (e.g. soy products (milk, yoghurt, cheese), coconut-, rice-, oat-, almond milk, cereal milk with soy), meat substitutes (e.g. tofu, tempeh, soy protein, vegetarian sausages), cereal substitutes (e.g. soy flour/flakes, lupines), sweeteners, sugar substitutes, beverage powders/ -granules (e.g. cocoa powder, lemonade powder), herbs, spices, vegetarian spreads, protein powder, yeast, miso</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Veg_products_NCI</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Vegetarian products</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Soyproducts_NCI</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Soyproducts</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>decimal</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Suessstoffe_MW</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
           <t>table sweeteners (low/no caloric sweeteners) (excl. Stevia)</t>
         </is>
       </c>
-      <c r="D57" t="inlineStr">
+      <c r="D61" t="inlineStr">
         <is>
           <t>decimal</t>
         </is>

</xml_diff>